<commit_message>
Changes for Accrual Balance Export
</commit_message>
<xml_diff>
--- a/bin/Debug/net6.0/LegionPayCodes.xlsx
+++ b/bin/Debug/net6.0/LegionPayCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emergere\ConnorsLLC\ConnorsLLC_Project\ProcessFiles_Demo\bin\Debug\net6.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FD914A-6E7B-4212-B9F2-77FD91179D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6052ED-21BA-473F-8BF3-C0A36DF2F4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="101">
   <si>
     <t>Pay Type</t>
   </si>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1077,15 +1077,13 @@
         <v>93</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="18" t="s">
-        <v>16</v>
+      <c r="C5" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>19</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E5" s="21"/>
       <c r="F5" s="10" t="s">
         <v>18</v>
       </c>

</xml_diff>